<commit_message>
Fix current and prior year headers in remaining QC town close workbooks
</commit_message>
<xml_diff>
--- a/dbt/export/templates/assessed_and_market_values.xlsx
+++ b/dbt/export/templates/assessed_and_market_values.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2568C871-9357-441A-B835-A5B7854C2CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9479033B-3F55-4D66-8D99-FB103B4D93C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="6180" windowWidth="28965" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,46 +37,46 @@
     <t>WHO</t>
   </si>
   <si>
-    <t>2023 LMV</t>
-  </si>
-  <si>
-    <t>2023 BMV</t>
-  </si>
-  <si>
-    <t>2023 Total MV</t>
-  </si>
-  <si>
-    <t>2023 LAV</t>
-  </si>
-  <si>
-    <t>2023 BAV</t>
-  </si>
-  <si>
-    <t>2023 Total AV</t>
-  </si>
-  <si>
-    <t>2024 LMV</t>
-  </si>
-  <si>
-    <t>2024 BMV</t>
-  </si>
-  <si>
-    <t>2024 Total MV</t>
-  </si>
-  <si>
-    <t>2024 LAV</t>
-  </si>
-  <si>
-    <t>2024 BAV</t>
-  </si>
-  <si>
-    <t>2024 Total AV</t>
-  </si>
-  <si>
     <t>TAXYR</t>
   </si>
   <si>
     <t>TOWNSHIP</t>
+  </si>
+  <si>
+    <t>Curr. Year LMV</t>
+  </si>
+  <si>
+    <t>Curr. Year BMV</t>
+  </si>
+  <si>
+    <t>Curr. Year Total MV</t>
+  </si>
+  <si>
+    <t>Curr. Year LAV</t>
+  </si>
+  <si>
+    <t>Curr. Year BAV</t>
+  </si>
+  <si>
+    <t>Curr. Year Total AV</t>
+  </si>
+  <si>
+    <t>Prior Year LMV</t>
+  </si>
+  <si>
+    <t>Prior Year BMV</t>
+  </si>
+  <si>
+    <t>Prior Year Total MV</t>
+  </si>
+  <si>
+    <t>Prior Year LAV</t>
+  </si>
+  <si>
+    <t>Prior Year BAV</t>
+  </si>
+  <si>
+    <t>Prior Year Total AV</t>
   </si>
 </sst>
 </file>
@@ -434,38 +434,38 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
-    <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="18.5546875" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+    <col min="19" max="19" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -480,40 +480,40 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix current and prior year headers in remaining QC town close workbooks (#837)
</commit_message>
<xml_diff>
--- a/dbt/export/templates/assessed_and_market_values.xlsx
+++ b/dbt/export/templates/assessed_and_market_values.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2568C871-9357-441A-B835-A5B7854C2CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9479033B-3F55-4D66-8D99-FB103B4D93C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="6180" windowWidth="28965" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,46 +37,46 @@
     <t>WHO</t>
   </si>
   <si>
-    <t>2023 LMV</t>
-  </si>
-  <si>
-    <t>2023 BMV</t>
-  </si>
-  <si>
-    <t>2023 Total MV</t>
-  </si>
-  <si>
-    <t>2023 LAV</t>
-  </si>
-  <si>
-    <t>2023 BAV</t>
-  </si>
-  <si>
-    <t>2023 Total AV</t>
-  </si>
-  <si>
-    <t>2024 LMV</t>
-  </si>
-  <si>
-    <t>2024 BMV</t>
-  </si>
-  <si>
-    <t>2024 Total MV</t>
-  </si>
-  <si>
-    <t>2024 LAV</t>
-  </si>
-  <si>
-    <t>2024 BAV</t>
-  </si>
-  <si>
-    <t>2024 Total AV</t>
-  </si>
-  <si>
     <t>TAXYR</t>
   </si>
   <si>
     <t>TOWNSHIP</t>
+  </si>
+  <si>
+    <t>Curr. Year LMV</t>
+  </si>
+  <si>
+    <t>Curr. Year BMV</t>
+  </si>
+  <si>
+    <t>Curr. Year Total MV</t>
+  </si>
+  <si>
+    <t>Curr. Year LAV</t>
+  </si>
+  <si>
+    <t>Curr. Year BAV</t>
+  </si>
+  <si>
+    <t>Curr. Year Total AV</t>
+  </si>
+  <si>
+    <t>Prior Year LMV</t>
+  </si>
+  <si>
+    <t>Prior Year BMV</t>
+  </si>
+  <si>
+    <t>Prior Year Total MV</t>
+  </si>
+  <si>
+    <t>Prior Year LAV</t>
+  </si>
+  <si>
+    <t>Prior Year BAV</t>
+  </si>
+  <si>
+    <t>Prior Year Total AV</t>
   </si>
 </sst>
 </file>
@@ -434,38 +434,38 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
-    <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="18.5546875" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+    <col min="19" max="19" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -480,40 +480,40 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>